<commit_message>
retraining scheme is working
</commit_message>
<xml_diff>
--- a/tickers1_sharpes.xlsx
+++ b/tickers1_sharpes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelmeisner/Desktop/5370/portfolio-opt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB001DAF-7677-DB4A-A69E-1A805DC69035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270BF4D3-30CB-8C4D-82CB-32115CB90CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{15A17078-C6AB-FE4B-9AF1-033A85536BF8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>LSTM</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Sharpe</t>
+  </si>
+  <si>
+    <t>LSTM w/ Retrain</t>
   </si>
 </sst>
 </file>
@@ -67,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -114,30 +117,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -155,7 +141,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="171" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -175,6 +161,23 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -189,10 +192,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BE99C15-B205-A149-BD05-438F17C90D17}" name="Table1" displayName="Table1" ref="C2:D8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BE99C15-B205-A149-BD05-438F17C90D17}" name="Table1" displayName="Table1" ref="C2:D9" totalsRowShown="0" headerRowDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4A3305B5-7449-E24C-BD0E-FBCF2533CBD6}" name="Portfolio" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4236D49A-D2CF-8945-BC9E-29A8C0C28AB0}" name="Sharpe" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4A3305B5-7449-E24C-BD0E-FBCF2533CBD6}" name="Portfolio" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{4236D49A-D2CF-8945-BC9E-29A8C0C28AB0}" name="Sharpe" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -515,13 +518,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28524D1-F017-044D-BD42-35A882E9D2E4}">
-  <dimension ref="C2:D8"/>
+  <dimension ref="C2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C2" sqref="C2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
@@ -533,54 +539,61 @@
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.100137968101239</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>5.9467218679682202E-2</v>
+        <v>0.100137968101239</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>5.1888653337151203E-2</v>
+        <v>5.9467218679682202E-2</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>4.9912275082059698E-2</v>
+        <v>5.1888653337151203E-2</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>3.9580144573736299E-2</v>
+        <v>4.9912275082059698E-2</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.9580144573736299E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>-1.8644236688449001E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>